<commit_message>
del duplicate (sorta) mwf template xlsx, fill in fields for remaining bwf template, add info for BWF file to field_mappings.json
</commit_message>
<xml_diff>
--- a/tests/AVMPI_Audio_BWF-EmbedMD_Guide_20240404.xlsx
+++ b/tests/AVMPI_Audio_BWF-EmbedMD_Guide_20240404.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet.sharepoint.com/sites/SI-AudiovisualMediaPreservationInitiative/Shared Documents/General/Workflows/Metadata/Embedded-Audio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcoates\code\avmpi_scripts\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69B93297-EE38-41E8-B8E5-7D0809209B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF2757-6979-4304-A81D-1E18646F00DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="760" windowWidth="33520" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields_InUse" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="159">
   <si>
     <t>Field</t>
   </si>
@@ -606,16 +606,106 @@
   <si>
     <t>FADGI Guidelines for Embedding Metadata</t>
   </si>
+  <si>
+    <t>SIA000485_A0001OM_01</t>
+  </si>
+  <si>
+    <t>unit_id, AC0509-OD0008;  avmpi_barcode, 31983000002816</t>
+  </si>
+  <si>
+    <t>Annual Convention: Omaha, Nebraska, Nov 1954 Tape 6</t>
+  </si>
+  <si>
+    <t>US, SI, NMAH-AC</t>
+  </si>
+  <si>
+    <t>US, SI, NMAI</t>
+  </si>
+  <si>
+    <t>AC0509-OD0008</t>
+  </si>
+  <si>
+    <t>010.001_AC0006</t>
+  </si>
+  <si>
+    <t>SIA000485_A0001OM</t>
+  </si>
+  <si>
+    <t>2023-12-16</t>
+  </si>
+  <si>
+    <t>2023-05-11</t>
+  </si>
+  <si>
+    <t>2024-03-26</t>
+  </si>
+  <si>
+    <t>11:00:14</t>
+  </si>
+  <si>
+    <t>2597547264</t>
+  </si>
+  <si>
+    <t>479329</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>060A2B340101010501010F1013000000CAB5703BEB8680000479C808F19818F0</t>
+  </si>
+  <si>
+    <t>1F913AC192FC4128AE42D77235A87F8A00000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>A=ANALOGUE, M=mono,T=EMT 927F; SME 3012R; ShureV15 TypeV; Endpoint preamp.  A=PCM,F=96000,W=24, M=mono,T=LavryGold AD122. A=PCM,F=96000,W=24,M=mono,T=ProTools v.2023.9</t>
+  </si>
+  <si>
+    <t>A=ANALOGUE,M=stereo,T=Tascam 122 MkII
+A=ANALOGUE,F=96000,W=24,M=stereo,T=Apogee Symphony I/O Mk II; SN001214001076</t>
+  </si>
+  <si>
+    <t>AVMPI</t>
+  </si>
+  <si>
+    <t>National Museum of American History. Division of Musical History</t>
+  </si>
+  <si>
+    <t>Severe plasticizer exudation required extensive cleaning. Moderate groove wear at head. Only side 1 recorded on disc</t>
+  </si>
+  <si>
+    <t>Copyright not evaluated.</t>
+  </si>
+  <si>
+    <t>DWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitch Your Wagon to a Star </t>
+  </si>
+  <si>
+    <t>Exhibit "This Thing Called Jazz"  Dec 1968-Jan 1969</t>
+  </si>
+  <si>
+    <t>Steinberg Cubase 12</t>
+  </si>
+  <si>
+    <t>Open-reel audiotape</t>
+  </si>
+  <si>
+    <t>AC0509-OD0008_01.wav</t>
+  </si>
+  <si>
+    <t>NMAI_010_33901000000364_p_01.wav</t>
+  </si>
+  <si>
+    <t>SIA000485_A0001OM_01.wav</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
-  </numFmts>
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1160,7 +1250,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1202,12 +1292,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="47" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="47" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1232,12 +1318,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1249,7 +1329,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -1273,9 +1367,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1313,7 +1407,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1419,7 +1513,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1561,7 +1655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1569,132 +1663,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08A5CA3-D756-BC46-B2B8-756B3D828B65}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="2" max="3" width="29.453125" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="54" customWidth="1"/>
+    <col min="5" max="5" width="31" style="54" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" customWidth="1"/>
+    <col min="7" max="7" width="27.26953125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="32" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="54" customWidth="1"/>
+    <col min="10" max="10" width="22.1796875" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" customWidth="1"/>
+    <col min="17" max="18" width="19.1796875" customWidth="1"/>
+    <col min="19" max="19" width="19.1796875" style="54" customWidth="1"/>
+    <col min="20" max="32" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="20" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:32" s="20" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="O1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="R1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="V1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="W1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="X1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Y1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="37" t="s">
+      <c r="AA1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="37" t="s">
+      <c r="AB1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="37" t="s">
+      <c r="AC1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="37" t="s">
+      <c r="AD1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="37" t="s">
+      <c r="AE1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="39" t="s">
+      <c r="AF1" s="37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="19" customFormat="1" ht="17.100000000000001" thickTop="1">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:32" s="19" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1703,10 +1800,10 @@
       <c r="C2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="51" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="22" t="s">
@@ -1718,7 +1815,7 @@
       <c r="H2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="57" t="s">
         <v>34</v>
       </c>
       <c r="J2" s="22" t="s">
@@ -1748,7 +1845,7 @@
       <c r="R2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="S2" s="51" t="s">
         <v>33</v>
       </c>
       <c r="T2" s="22" t="s">
@@ -1787,12 +1884,12 @@
       <c r="AE2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="41" t="s">
+      <c r="AF2" s="39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="134.1" customHeight="1">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:32" ht="134.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="40" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -1801,31 +1898,31 @@
       <c r="C3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="52">
         <v>45014</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="55">
         <v>0.60428240740740746</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30">
+      <c r="G3" s="30"/>
+      <c r="H3" s="29">
         <v>2</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="58">
         <v>0</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="30" t="s">
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="29" t="s">
         <v>41</v>
       </c>
       <c r="Q3" s="28" t="s">
@@ -1834,135 +1931,267 @@
       <c r="R3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="29">
+      <c r="S3" s="52">
         <v>45014</v>
       </c>
       <c r="T3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="34" t="s">
+      <c r="U3" s="29"/>
+      <c r="V3" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
       <c r="Z3" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="30" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="30" t="s">
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AF3" s="43" t="s">
+      <c r="AF3" s="41" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="18" customFormat="1" ht="408.95" customHeight="1" thickBot="1">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:32" s="18" customFormat="1" ht="409" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="Q4" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="S4" s="45" t="s">
+      <c r="S4" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="T4" s="45" t="s">
+      <c r="T4" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="U4" s="45" t="s">
+      <c r="U4" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="V4" s="49" t="s">
+      <c r="V4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="W4" s="53" t="s">
+      <c r="W4" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="X4" s="50" t="s">
+      <c r="X4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="Y4" s="50" t="s">
+      <c r="Y4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="Z4" s="45" t="s">
+      <c r="Z4" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="AA4" s="45" t="s">
+      <c r="AA4" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="AB4" s="45" t="s">
+      <c r="AB4" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="AC4" s="46" t="s">
+      <c r="AC4" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD4" s="45" t="s">
+      <c r="AD4" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="AE4" s="45" t="s">
+      <c r="AE4" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="AF4" s="51" t="s">
+      <c r="AF4" s="47" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S5" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="T5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" t="s">
+        <v>150</v>
+      </c>
+      <c r="T6" t="s">
+        <v>130</v>
+      </c>
+      <c r="W6" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" t="s">
+        <v>150</v>
+      </c>
+      <c r="T7" t="s">
+        <v>153</v>
+      </c>
+      <c r="U7" t="s">
+        <v>148</v>
+      </c>
+      <c r="W7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1978,15 +2207,15 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" customWidth="1"/>
+    <col min="3" max="3" width="61.453125" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -2000,7 +2229,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -2014,7 +2243,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
@@ -2028,7 +2257,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33.950000000000003">
+    <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>80</v>
       </c>
@@ -2042,7 +2271,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="51">
+    <row r="5" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
@@ -2056,7 +2285,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33.950000000000003">
+    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
@@ -2070,7 +2299,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="68.099999999999994">
+    <row r="7" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
@@ -2084,7 +2313,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.100000000000001">
+    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>80</v>
       </c>
@@ -2098,7 +2327,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33.950000000000003">
+    <row r="9" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>80</v>
       </c>
@@ -2112,7 +2341,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>80</v>
       </c>
@@ -2126,7 +2355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="33.950000000000003">
+    <row r="11" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -2140,7 +2369,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="33.950000000000003">
+    <row r="12" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>80</v>
       </c>
@@ -2154,7 +2383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33.950000000000003">
+    <row r="13" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>80</v>
       </c>
@@ -2168,7 +2397,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="33.950000000000003">
+    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>80</v>
       </c>
@@ -2182,7 +2411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="33.950000000000003">
+    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>80</v>
       </c>
@@ -2196,7 +2425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.100000000000001">
+    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -2210,7 +2439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.100000000000001">
+    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>99</v>
       </c>
@@ -2224,7 +2453,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="33.950000000000003">
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>99</v>
       </c>
@@ -2238,7 +2467,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.100000000000001">
+    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>99</v>
       </c>
@@ -2252,7 +2481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.100000000000001">
+    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>99</v>
       </c>
@@ -2266,7 +2495,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="33.950000000000003">
+    <row r="21" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>99</v>
       </c>
@@ -2280,7 +2509,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.100000000000001">
+    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>99</v>
       </c>
@@ -2294,7 +2523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.100000000000001">
+    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>99</v>
       </c>
@@ -2308,7 +2537,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.100000000000001">
+    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>99</v>
       </c>
@@ -2322,7 +2551,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.100000000000001">
+    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>99</v>
       </c>
@@ -2336,7 +2565,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.100000000000001">
+    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>99</v>
       </c>
@@ -2350,7 +2579,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.100000000000001">
+    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>99</v>
       </c>
@@ -2364,7 +2593,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.100000000000001">
+    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>99</v>
       </c>
@@ -2378,7 +2607,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.100000000000001">
+    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>99</v>
       </c>
@@ -2392,7 +2621,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="51">
+    <row r="30" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>99</v>
       </c>
@@ -2406,7 +2635,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.100000000000001">
+    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
@@ -2420,7 +2649,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.100000000000001">
+    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>99</v>
       </c>
@@ -2447,13 +2676,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>117</v>
       </c>
@@ -2461,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>118</v>
       </c>
@@ -2469,7 +2698,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>120</v>
       </c>
@@ -2477,7 +2706,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>122</v>
       </c>
@@ -2485,7 +2714,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>124</v>
       </c>
@@ -2493,7 +2722,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>126</v>
       </c>
@@ -2514,21 +2743,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ddba8c88-3c65-4e0a-a7e6-1225a6414a49">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="429e945e-0d47-4333-a662-93795e49a0fb" xsi:nil="true"/>
-    <SharedWithUsers xmlns="429e945e-0d47-4333-a662-93795e49a0fb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2787,22 +3007,57 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ddba8c88-3c65-4e0a-a7e6-1225a6414a49">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="429e945e-0d47-4333-a662-93795e49a0fb" xsi:nil="true"/>
+    <SharedWithUsers xmlns="429e945e-0d47-4333-a662-93795e49a0fb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DD296B5-5C91-4245-AAB5-DB6AF40ED322}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B443D2-0FAD-4544-B174-546F40647206}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99F06AB-5B5F-4664-91F3-D63BD3159064}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99F06AB-5B5F-4664-91F3-D63BD3159064}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ddba8c88-3c65-4e0a-a7e6-1225a6414a49"/>
+    <ds:schemaRef ds:uri="429e945e-0d47-4333-a662-93795e49a0fb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B443D2-0FAD-4544-B174-546F40647206}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DD296B5-5C91-4245-AAB5-DB6AF40ED322}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ddba8c88-3c65-4e0a-a7e6-1225a6414a49"/>
+    <ds:schemaRef ds:uri="429e945e-0d47-4333-a662-93795e49a0fb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>